<commit_message>
till vidoe 87 done
</commit_message>
<xml_diff>
--- a/Sigma Web Development Course - Web Development Tutorials in Hindi 🗿 (1).xlsx
+++ b/Sigma Web Development Course - Web Development Tutorials in Hindi 🗿 (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayav\Desktop\Sigma Web Dev Course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAAEC4E-D8F2-42CB-8D81-A9F146BF7DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45C8610-C4E4-4F86-A06D-6A7DE4554055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Playlist data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="770">
   <si>
     <t>Title</t>
   </si>
@@ -6950,21 +6950,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K164"/>
+  <dimension ref="A1:K191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C164" sqref="C164"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C167" sqref="C167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.100000000000001" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="87" customWidth="1"/>
-    <col min="3" max="3" width="40.81640625" customWidth="1"/>
-    <col min="9" max="9" width="34.81640625" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="91.25" customWidth="1"/>
+    <col min="3" max="3" width="30.5" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
+    <col min="9" max="9" width="34.875" customWidth="1"/>
+    <col min="11" max="11" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6999,7 +7001,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7034,7 +7036,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -7069,7 +7071,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -7104,7 +7106,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -7139,7 +7141,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -7174,7 +7176,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -7209,7 +7211,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -7244,7 +7246,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -7279,7 +7281,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -7314,7 +7316,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -7349,7 +7351,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -7384,7 +7386,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>78</v>
       </c>
@@ -7419,7 +7421,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -7454,7 +7456,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -7489,7 +7491,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>96</v>
       </c>
@@ -7524,7 +7526,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -7559,7 +7561,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>108</v>
       </c>
@@ -7594,7 +7596,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>114</v>
       </c>
@@ -7629,7 +7631,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>120</v>
       </c>
@@ -7664,7 +7666,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -7699,7 +7701,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>132</v>
       </c>
@@ -7734,7 +7736,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>138</v>
       </c>
@@ -7769,7 +7771,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>144</v>
       </c>
@@ -7804,7 +7806,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>150</v>
       </c>
@@ -7839,7 +7841,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>156</v>
       </c>
@@ -7874,7 +7876,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>162</v>
       </c>
@@ -7909,7 +7911,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>168</v>
       </c>
@@ -7944,7 +7946,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>174</v>
       </c>
@@ -7979,7 +7981,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>180</v>
       </c>
@@ -8014,7 +8016,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>186</v>
       </c>
@@ -8049,7 +8051,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>191</v>
       </c>
@@ -8084,7 +8086,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>196</v>
       </c>
@@ -8119,7 +8121,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>202</v>
       </c>
@@ -8154,7 +8156,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>207</v>
       </c>
@@ -8189,7 +8191,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>211</v>
       </c>
@@ -8224,7 +8226,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>216</v>
       </c>
@@ -8259,7 +8261,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>221</v>
       </c>
@@ -8294,7 +8296,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>226</v>
       </c>
@@ -8329,7 +8331,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>232</v>
       </c>
@@ -8364,7 +8366,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>238</v>
       </c>
@@ -8399,7 +8401,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>243</v>
       </c>
@@ -8434,7 +8436,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>249</v>
       </c>
@@ -8469,7 +8471,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>255</v>
       </c>
@@ -8504,7 +8506,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>261</v>
       </c>
@@ -8539,7 +8541,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>267</v>
       </c>
@@ -8574,7 +8576,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>273</v>
       </c>
@@ -8609,7 +8611,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>279</v>
       </c>
@@ -8644,7 +8646,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>285</v>
       </c>
@@ -8679,7 +8681,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>291</v>
       </c>
@@ -8714,7 +8716,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>297</v>
       </c>
@@ -8749,7 +8751,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>303</v>
       </c>
@@ -8784,7 +8786,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>309</v>
       </c>
@@ -8819,7 +8821,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>315</v>
       </c>
@@ -8854,7 +8856,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>321</v>
       </c>
@@ -8889,7 +8891,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>327</v>
       </c>
@@ -8924,7 +8926,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>333</v>
       </c>
@@ -8959,7 +8961,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>339</v>
       </c>
@@ -8994,7 +8996,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>345</v>
       </c>
@@ -9029,7 +9031,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>351</v>
       </c>
@@ -9064,7 +9066,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>357</v>
       </c>
@@ -9099,7 +9101,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>363</v>
       </c>
@@ -9134,7 +9136,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>369</v>
       </c>
@@ -9169,7 +9171,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>374</v>
       </c>
@@ -9204,7 +9206,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>379</v>
       </c>
@@ -9239,7 +9241,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>384</v>
       </c>
@@ -9274,7 +9276,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>389</v>
       </c>
@@ -9309,7 +9311,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>394</v>
       </c>
@@ -9344,7 +9346,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>400</v>
       </c>
@@ -9379,7 +9381,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>405</v>
       </c>
@@ -9414,7 +9416,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>410</v>
       </c>
@@ -9449,7 +9451,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>415</v>
       </c>
@@ -9484,7 +9486,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>420</v>
       </c>
@@ -9519,7 +9521,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>425</v>
       </c>
@@ -9554,7 +9556,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>430</v>
       </c>
@@ -9589,7 +9591,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>435</v>
       </c>
@@ -9624,7 +9626,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>440</v>
       </c>
@@ -9659,7 +9661,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>445</v>
       </c>
@@ -9694,7 +9696,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>450</v>
       </c>
@@ -9729,7 +9731,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>454</v>
       </c>
@@ -9764,7 +9766,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>459</v>
       </c>
@@ -9799,7 +9801,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>464</v>
       </c>
@@ -9834,7 +9836,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>469</v>
       </c>
@@ -9869,7 +9871,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>474</v>
       </c>
@@ -9904,7 +9906,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>479</v>
       </c>
@@ -9939,7 +9941,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>485</v>
       </c>
@@ -9974,7 +9976,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>490</v>
       </c>
@@ -10009,7 +10011,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>495</v>
       </c>
@@ -10044,7 +10046,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>501</v>
       </c>
@@ -10079,7 +10081,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>506</v>
       </c>
@@ -10114,7 +10116,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>511</v>
       </c>
@@ -10149,7 +10151,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>516</v>
       </c>
@@ -10184,7 +10186,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>521</v>
       </c>
@@ -10219,7 +10221,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>526</v>
       </c>
@@ -10254,7 +10256,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>531</v>
       </c>
@@ -10289,7 +10291,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>536</v>
       </c>
@@ -10324,7 +10326,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>541</v>
       </c>
@@ -10359,7 +10361,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>546</v>
       </c>
@@ -10394,7 +10396,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>551</v>
       </c>
@@ -10429,7 +10431,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>557</v>
       </c>
@@ -10464,7 +10466,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>563</v>
       </c>
@@ -10499,7 +10501,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>569</v>
       </c>
@@ -10534,7 +10536,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>575</v>
       </c>
@@ -10569,7 +10571,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>580</v>
       </c>
@@ -10604,7 +10606,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>586</v>
       </c>
@@ -10639,7 +10641,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>592</v>
       </c>
@@ -10674,7 +10676,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>598</v>
       </c>
@@ -10709,7 +10711,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>603</v>
       </c>
@@ -10744,7 +10746,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>608</v>
       </c>
@@ -10779,7 +10781,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>613</v>
       </c>
@@ -10814,7 +10816,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>618</v>
       </c>
@@ -10849,7 +10851,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>624</v>
       </c>
@@ -10884,7 +10886,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>629</v>
       </c>
@@ -10919,7 +10921,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>635</v>
       </c>
@@ -10954,7 +10956,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>640</v>
       </c>
@@ -10989,7 +10991,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>645</v>
       </c>
@@ -11024,7 +11026,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>650</v>
       </c>
@@ -11059,7 +11061,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>655</v>
       </c>
@@ -11094,7 +11096,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>660</v>
       </c>
@@ -11129,7 +11131,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>664</v>
       </c>
@@ -11164,7 +11166,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>669</v>
       </c>
@@ -11199,7 +11201,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>674</v>
       </c>
@@ -11234,7 +11236,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>679</v>
       </c>
@@ -11269,7 +11271,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>683</v>
       </c>
@@ -11304,7 +11306,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>688</v>
       </c>
@@ -11339,7 +11341,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>693</v>
       </c>
@@ -11374,7 +11376,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>697</v>
       </c>
@@ -11409,7 +11411,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>702</v>
       </c>
@@ -11444,7 +11446,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>707</v>
       </c>
@@ -11479,7 +11481,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>712</v>
       </c>
@@ -11514,7 +11516,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>717</v>
       </c>
@@ -11549,7 +11551,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>723</v>
       </c>
@@ -11584,7 +11586,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>729</v>
       </c>
@@ -11619,7 +11621,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>734</v>
       </c>
@@ -11654,7 +11656,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>739</v>
       </c>
@@ -11689,7 +11691,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>744</v>
       </c>
@@ -11724,7 +11726,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>749</v>
       </c>
@@ -11759,7 +11761,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>754</v>
       </c>
@@ -11794,7 +11796,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>759</v>
       </c>
@@ -11829,7 +11831,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>764</v>
       </c>
@@ -11864,7 +11866,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>1</v>
       </c>
@@ -11875,7 +11877,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>2</v>
       </c>
@@ -11886,7 +11888,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>3</v>
       </c>
@@ -11897,7 +11899,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>4</v>
       </c>
@@ -11908,7 +11910,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>5</v>
       </c>
@@ -11919,7 +11921,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>6</v>
       </c>
@@ -11930,7 +11932,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>7</v>
       </c>
@@ -11941,7 +11943,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>8</v>
       </c>
@@ -11952,7 +11954,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>9</v>
       </c>
@@ -11963,7 +11965,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>10</v>
       </c>
@@ -11974,7 +11976,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>11</v>
       </c>
@@ -11985,7 +11987,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>12</v>
       </c>
@@ -11996,7 +11998,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>13</v>
       </c>
@@ -12007,7 +12009,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>14</v>
       </c>
@@ -12018,7 +12020,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>15</v>
       </c>
@@ -12029,7 +12031,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>16</v>
       </c>
@@ -12040,7 +12042,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>17</v>
       </c>
@@ -12051,7 +12053,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>18</v>
       </c>
@@ -12062,7 +12064,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>19</v>
       </c>
@@ -12071,6 +12073,272 @@
       </c>
       <c r="C164" t="s">
         <v>767</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>1</v>
+      </c>
+      <c r="B171" t="s">
+        <v>485</v>
+      </c>
+      <c r="C171" t="s">
+        <v>487</v>
+      </c>
+      <c r="D171" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>2</v>
+      </c>
+      <c r="B172" t="s">
+        <v>490</v>
+      </c>
+      <c r="C172" t="s">
+        <v>492</v>
+      </c>
+      <c r="D172" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>3</v>
+      </c>
+      <c r="B173" t="s">
+        <v>495</v>
+      </c>
+      <c r="C173" t="s">
+        <v>498</v>
+      </c>
+      <c r="D173" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>4</v>
+      </c>
+      <c r="B174" t="s">
+        <v>501</v>
+      </c>
+      <c r="C174" t="s">
+        <v>503</v>
+      </c>
+      <c r="D174" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>5</v>
+      </c>
+      <c r="B175" t="s">
+        <v>506</v>
+      </c>
+      <c r="C175" t="s">
+        <v>508</v>
+      </c>
+      <c r="D175" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>6</v>
+      </c>
+      <c r="B176" t="s">
+        <v>511</v>
+      </c>
+      <c r="C176" t="s">
+        <v>513</v>
+      </c>
+      <c r="D176" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>7</v>
+      </c>
+      <c r="B177" t="s">
+        <v>516</v>
+      </c>
+      <c r="C177" t="s">
+        <v>518</v>
+      </c>
+      <c r="D177" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>8</v>
+      </c>
+      <c r="B178" t="s">
+        <v>521</v>
+      </c>
+      <c r="C178" t="s">
+        <v>523</v>
+      </c>
+      <c r="D178" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>9</v>
+      </c>
+      <c r="B179" t="s">
+        <v>526</v>
+      </c>
+      <c r="C179" t="s">
+        <v>528</v>
+      </c>
+      <c r="D179" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>10</v>
+      </c>
+      <c r="B180" t="s">
+        <v>531</v>
+      </c>
+      <c r="C180" t="s">
+        <v>533</v>
+      </c>
+      <c r="D180" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>11</v>
+      </c>
+      <c r="B181" t="s">
+        <v>536</v>
+      </c>
+      <c r="C181" t="s">
+        <v>538</v>
+      </c>
+      <c r="D181" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>12</v>
+      </c>
+      <c r="B182" t="s">
+        <v>541</v>
+      </c>
+      <c r="C182" t="s">
+        <v>543</v>
+      </c>
+      <c r="D182" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>13</v>
+      </c>
+      <c r="B183" t="s">
+        <v>546</v>
+      </c>
+      <c r="C183" t="s">
+        <v>548</v>
+      </c>
+      <c r="D183" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>14</v>
+      </c>
+      <c r="B184" t="s">
+        <v>557</v>
+      </c>
+      <c r="C184" t="s">
+        <v>560</v>
+      </c>
+      <c r="D184" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>15</v>
+      </c>
+      <c r="B185" t="s">
+        <v>563</v>
+      </c>
+      <c r="C185" t="s">
+        <v>566</v>
+      </c>
+      <c r="D185" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>16</v>
+      </c>
+      <c r="B188" t="s">
+        <v>569</v>
+      </c>
+      <c r="C188" t="s">
+        <v>572</v>
+      </c>
+      <c r="D188" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>17</v>
+      </c>
+      <c r="B189" t="s">
+        <v>575</v>
+      </c>
+      <c r="C189" t="s">
+        <v>577</v>
+      </c>
+      <c r="D189" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>18</v>
+      </c>
+      <c r="B190" t="s">
+        <v>580</v>
+      </c>
+      <c r="C190" t="s">
+        <v>583</v>
+      </c>
+      <c r="D190" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>19</v>
+      </c>
+      <c r="B191" t="s">
+        <v>586</v>
+      </c>
+      <c r="C191" t="s">
+        <v>589</v>
+      </c>
+      <c r="D191" t="s">
+        <v>591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>